<commit_message>
swapped spreadsheet 2D array for DataSet
</commit_message>
<xml_diff>
--- a/wwwroot/spreadsheets/spreadsheet.xlsx
+++ b/wwwroot/spreadsheets/spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A3D9536-D3B4-4E91-9090-5B87E23C5EE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E7294BE-033A-46BB-BFFE-4F0D4EC492F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5715" yWindow="5505" windowWidth="28800" windowHeight="15885" xr2:uid="{9512FE5E-EFC2-4215-BB83-A761C78B376D}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>firstname</t>
   </si>
@@ -57,6 +57,24 @@
   </si>
   <si>
     <t>frank@email.com</t>
+  </si>
+  <si>
+    <t>dylan</t>
+  </si>
+  <si>
+    <t>dylan@email.com</t>
+  </si>
+  <si>
+    <t>melbourne</t>
+  </si>
+  <si>
+    <t>eric</t>
+  </si>
+  <si>
+    <t>eric@email.com</t>
+  </si>
+  <si>
+    <t>brisbane</t>
   </si>
 </sst>
 </file>
@@ -419,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC4DDDD2-9AF7-49A2-A073-6BE829E487BB}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,10 +478,34 @@
         <v>5</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{39DD94E4-D4ED-4E2B-AE5F-5E8D4C061892}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{6F0DE82F-B3D9-49AB-9467-5700F6C9FBB8}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{935EC069-E750-457A-8F10-FA4C0CD6BF5F}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{E96515EA-EB70-4667-BBB5-08B1CDF6BE6E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Setup outlook auth. Functionality to send email finished
</commit_message>
<xml_diff>
--- a/wwwroot/spreadsheets/spreadsheet.xlsx
+++ b/wwwroot/spreadsheets/spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E7294BE-033A-46BB-BFFE-4F0D4EC492F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{190DE441-F089-4F48-AFFA-B3DB3B1B0235}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5715" yWindow="5505" windowWidth="28800" windowHeight="15885" xr2:uid="{9512FE5E-EFC2-4215-BB83-A761C78B376D}"/>
+    <workbookView xWindow="420" yWindow="315" windowWidth="28800" windowHeight="15885" xr2:uid="{9512FE5E-EFC2-4215-BB83-A761C78B376D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,34 +47,34 @@
     <t>bob</t>
   </si>
   <si>
+    <t>sydney</t>
+  </si>
+  <si>
+    <t>frank</t>
+  </si>
+  <si>
+    <t>frank@email.com</t>
+  </si>
+  <si>
+    <t>dylan</t>
+  </si>
+  <si>
+    <t>dylan@email.com</t>
+  </si>
+  <si>
+    <t>melbourne</t>
+  </si>
+  <si>
+    <t>eric</t>
+  </si>
+  <si>
+    <t>eric@email.com</t>
+  </si>
+  <si>
+    <t>brisbane</t>
+  </si>
+  <si>
     <t>bob@email.com</t>
-  </si>
-  <si>
-    <t>sydney</t>
-  </si>
-  <si>
-    <t>frank</t>
-  </si>
-  <si>
-    <t>frank@email.com</t>
-  </si>
-  <si>
-    <t>dylan</t>
-  </si>
-  <si>
-    <t>dylan@email.com</t>
-  </si>
-  <si>
-    <t>melbourne</t>
-  </si>
-  <si>
-    <t>eric</t>
-  </si>
-  <si>
-    <t>eric@email.com</t>
-  </si>
-  <si>
-    <t>brisbane</t>
   </si>
 </sst>
 </file>
@@ -461,51 +461,51 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" t="s">
         <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" t="s">
         <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{39DD94E4-D4ED-4E2B-AE5F-5E8D4C061892}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{6F0DE82F-B3D9-49AB-9467-5700F6C9FBB8}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{935EC069-E750-457A-8F10-FA4C0CD6BF5F}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{E96515EA-EB70-4667-BBB5-08B1CDF6BE6E}"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{6F0DE82F-B3D9-49AB-9467-5700F6C9FBB8}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{935EC069-E750-457A-8F10-FA4C0CD6BF5F}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{E96515EA-EB70-4667-BBB5-08B1CDF6BE6E}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{46748774-FBB6-447A-B4BA-5B6CDF83C175}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
cleaned up message configuration
</commit_message>
<xml_diff>
--- a/wwwroot/spreadsheets/spreadsheet.xlsx
+++ b/wwwroot/spreadsheets/spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{190DE441-F089-4F48-AFFA-B3DB3B1B0235}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D15B971-3BFA-4811-A2DB-F38F9A28D747}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="315" windowWidth="28800" windowHeight="15885" xr2:uid="{9512FE5E-EFC2-4215-BB83-A761C78B376D}"/>
+    <workbookView xWindow="3345" yWindow="2805" windowWidth="28800" windowHeight="15885" xr2:uid="{9512FE5E-EFC2-4215-BB83-A761C78B376D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>firstname</t>
   </si>
@@ -53,35 +53,26 @@
     <t>frank</t>
   </si>
   <si>
-    <t>frank@email.com</t>
-  </si>
-  <si>
     <t>dylan</t>
   </si>
   <si>
-    <t>dylan@email.com</t>
-  </si>
-  <si>
     <t>melbourne</t>
   </si>
   <si>
     <t>eric</t>
   </si>
   <si>
-    <t>eric@email.com</t>
-  </si>
-  <si>
     <t>brisbane</t>
   </si>
   <si>
-    <t>bob@email.com</t>
+    <t>thunderchunderthrowaway@outlook.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,6 +87,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -119,9 +116,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -440,7 +440,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,7 +461,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -471,8 +471,8 @@
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -480,33 +480,31 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{6F0DE82F-B3D9-49AB-9467-5700F6C9FBB8}"/>
-    <hyperlink ref="B4" r:id="rId2" xr:uid="{935EC069-E750-457A-8F10-FA4C0CD6BF5F}"/>
-    <hyperlink ref="B5" r:id="rId3" xr:uid="{E96515EA-EB70-4667-BBB5-08B1CDF6BE6E}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{46748774-FBB6-447A-B4BA-5B6CDF83C175}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{46748774-FBB6-447A-B4BA-5B6CDF83C175}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>